<commit_message>
& - 24856 от 16.12.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC.xlsx
+++ b/Collections/EURO/Andorra/#EURO#Andorra#Commemorative#[2014-present]#UNC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Andorra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1B3468-26DE-4442-B1F6-DE2C288569EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDD091D-B1C5-4CC1-8880-2A4F07386936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -112,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -289,6 +292,15 @@
   </si>
   <si>
     <t>6th page</t>
+  </si>
+  <si>
+    <t>Games of the Small States of Europe 2025</t>
+  </si>
+  <si>
+    <t>Bearded Vulture</t>
+  </si>
+  <si>
+    <t>60.000</t>
   </si>
 </sst>
 </file>
@@ -916,7 +928,31 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="33">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1163,9 +1199,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="4" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1440,7 +1476,7 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2197,13 +2233,59 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="14">
+        <v>64000</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="24">
+        <v>1</v>
+      </c>
       <c r="J24" s="62"/>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
+      <c r="A25" s="6">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="24">
+        <v>1</v>
+      </c>
       <c r="J25" s="62"/>
       <c r="K25"/>
     </row>
@@ -2219,11 +2301,45 @@
     <mergeCell ref="C1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H5 H8:H9 H12:H13">
-    <cfRule type="containsText" dxfId="29" priority="101" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="32" priority="107" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H5 H8:H9 H12:H13">
+    <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3 I6:I7 I10:I11">
+    <cfRule type="containsText" dxfId="31" priority="105" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I7 I3 I10:I11">
+    <cfRule type="colorScale" priority="106">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
+    <cfRule type="containsText" dxfId="30" priority="101" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
     <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2235,12 +2351,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3 I6:I7 I10:I11">
-    <cfRule type="containsText" dxfId="28" priority="99" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I7 I3 I10:I11">
+  <conditionalFormatting sqref="H16:H17">
+    <cfRule type="containsText" dxfId="29" priority="99" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:H17">
     <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2252,29 +2368,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
-    <cfRule type="containsText" dxfId="27" priority="95" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
-    <cfRule type="colorScale" priority="96">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H17">
-    <cfRule type="containsText" dxfId="26" priority="93" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H17">
+  <conditionalFormatting sqref="I18:I19">
+    <cfRule type="containsText" dxfId="28" priority="93" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:I19">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2286,13 +2385,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I19">
-    <cfRule type="containsText" dxfId="25" priority="87" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I19">
-    <cfRule type="colorScale" priority="88">
+  <conditionalFormatting sqref="H20:H21">
+    <cfRule type="containsText" dxfId="27" priority="91" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:H21">
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2303,13 +2402,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H21">
-    <cfRule type="containsText" dxfId="24" priority="85" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H21">
-    <cfRule type="colorScale" priority="86">
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="containsText" dxfId="26" priority="47" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2320,12 +2419,46 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="containsText" dxfId="25" priority="45" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="containsText" dxfId="24" priority="43" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
     <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2337,12 +2470,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I8">
     <cfRule type="containsText" dxfId="22" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I5))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2354,12 +2487,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I9">
     <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2371,12 +2504,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H10">
     <cfRule type="containsText" dxfId="20" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2388,12 +2521,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="H11">
     <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2405,12 +2538,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+  <conditionalFormatting sqref="H14">
     <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2422,12 +2555,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="H15">
     <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2439,12 +2572,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="I12">
     <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2456,12 +2589,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="I13">
     <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2473,12 +2606,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2490,12 +2623,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="I17">
     <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2507,12 +2640,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+  <conditionalFormatting sqref="H18">
     <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2524,12 +2657,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="H19">
     <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2541,12 +2674,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="I20">
     <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2558,12 +2691,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="I21">
     <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I21))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2575,12 +2708,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="I22:I23">
     <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I23">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2592,12 +2725,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="H22">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2609,12 +2742,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="H23">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I21))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2626,12 +2759,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I23">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I23">
+  <conditionalFormatting sqref="H24:H25">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:H25">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2643,12 +2776,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="I24">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2660,12 +2793,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="I25">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I25))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2688,7 +2821,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>